<commit_message>
Adding slippage, commissions, volume threshold
</commit_message>
<xml_diff>
--- a/Variable_list.xlsx
+++ b/Variable_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavan\Valkyrie\engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA76A06-F604-49D7-BB41-1F482C76458A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55E2BA9-4ECC-4260-8AC1-5A8A4C8DA022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Close</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Fama_French</t>
+  </si>
+  <si>
+    <t>ADV</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -679,6 +682,11 @@
         <v>39</v>
       </c>
     </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>